<commit_message>
problema giocatori e test altri classifier
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Desktop/All/Database/AnalyzeFootball/FantasyFootball/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vittu\Documents\Stupido\Betting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8C13D8-5199-3840-B5CA-1D18BDFBF477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E155EE-F8CF-41D8-85B8-E6919F852DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3588" yWindow="3588" windowWidth="14892" windowHeight="7716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
   <si>
     <t>ATALANTAOpponent</t>
   </si>
@@ -615,15 +615,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -870,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1743,6 +1743,131 @@
       </c>
       <c r="AO9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>53</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10" t="s">
+        <v>59</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ultimo aggiornamento prima di nuovo setup fatto da Peter
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vittu\Documents\Stupido\Betting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E155EE-F8CF-41D8-85B8-E6919F852DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43266810-0D31-4EF4-9DFF-1E86D63C1580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3588" yWindow="3588" windowWidth="14892" windowHeight="7716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="60">
   <si>
     <t>ATALANTAOpponent</t>
   </si>
@@ -269,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -277,6 +277,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,13 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO10"/>
+  <dimension ref="A1:AO37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="41" width="15.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -1870,7 +1874,503 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" t="s">
+        <v>44</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>56</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>49</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
+        <v>52</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK12">
+        <v>1</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>55</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>